<commit_message>
Summarizes RSP into excel
</commit_message>
<xml_diff>
--- a/data/RSP_Rookies.xlsx
+++ b/data/RSP_Rookies.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="152" documentId="8_{0EB90C79-FC22-4A12-A94D-9985B2A593C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC2149D-B560-42B1-93F7-9F725FF0DCA1}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{0EB90C79-FC22-4A12-A94D-9985B2A593C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06E58B38-EF1A-45B1-B827-5316FD62CDB8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="38020" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$50</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="216">
   <si>
     <t>Player</t>
   </si>
@@ -777,6 +777,682 @@
 Player Comparisons:
 J.K. Dobbins / Khalil Herbert: These comparisons suggest potential as an efficient, explosive runner often effective in zone schemes, likely fitting best within a committee approach.
 Bottom Line for Rookie Drafts: Hunter is a physically gifted back with the raw tools to succeed, particularly fitting a zone-running scheme. His blend of speed and power offers upside. However, the need for significant technical refinement in receiving, pass protection, and decision-making in certain run concepts makes him more of a developmental prospect than a finished product. He projects as a committee back who could offer splash weeks if he earns a role. The RSP evaluator suggests he's worth stashing (Rounds 3-4+ value in rookie drafts), betting on his athletic ability and potential for rapid development with NFL coaching.</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>X/Brandon Aiyuk – Rashee Rice - Dontayvion Wicks/Quintez Cephus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Franchise: Challenging for the lead role and leadership anchor. </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Luther Burden III grades out as the RSP WR1 and a "Franchise" level talent, projected for immediate high-level production in the NFL. The evaluator holds him in exceptionally high regard, suggesting he would have ranked Burden ahead of Marvin Harrison Jr. pre-draft last year. Burden is lauded as a highly versatile, athletic receiver whose superpower is his elite ability after the catch ("one of the two best runners... in this receiver class"). While needing refinement in his releases against press coverage and as a blocker, his combination of speed, elite short-area quickness, reliable hands, route savvy, and football IQ points towards a potential alpha receiver profile. He's strongly recommended as a top-3 rookie pick, regardless of landing spot.
+Fantasy Strengths:
+Elite After-the-Catch Ability: Exceptional vision, patience, elite short-area quickness, power, balance, and a diverse repertoire of moves make him incredibly dangerous with the ball in his hands. Creates yards and touchdowns independently.
+Versatility: Can effectively play all three wide receiver positions (slot, flanker, potentially X with development) and contribute on various routes (vertical, crossers, screens) and manufactured touches (sweeps).
+Athleticism: Possesses difference-making speed to win deep or pull away after the catch, combined with elite quickness and deceleration for separation and YAC.
+Reliable Hands &amp; Catching: Excellent catch reliability (100% pinpoint catch rate in tracked games), tracks the ball well (over-shoulder, adjusting to placement), extends effectively, uses his body well, and makes contested/difficult catches (including one-handed grabs).
+Route Running &amp; Football IQ: Understands how to attack zone coverage, tempos routes effectively, works the scramble drill intelligently, and shows nuance in stems and breaks (though limited exposure to hard comeback routes). High football IQ evident in his play.
+Good Ball Security &amp; Durability: Generally takes care of the football and has no significant injury history reported.
+Fantasy Weaknesses:
+Release vs. Press Coverage: Needs to refine the pacing and artistry of his release packages to consistently defeat top-tier press corners at the line of scrimmage. This is the primary area holding him back from being a dominant 'X' receiver immediately.
+Blocking Technique: Requires significant improvement in technique (closing distance, punch timing/force, avoiding overextension) to become a reliable blocker.
+Catching Technique (Minor): Hands could be slightly tighter on occasion when attacking the ball to prevent potential issues against NFL velocity (though drops weren't observed).
+Player Comparisons:
+Spectrum includes Brandon Aiyuk, Rashee Rice, Dontayvion Wicks, Quintez Cephus.
+The Brandon Aiyuk comparison aligns well with Burden's profile as a versatile, explosive receiver who excels after the catch and can win at multiple levels. Rashee Rice highlights the YAC prowess and potential slot/intermediate effectiveness.
+Bottom Line for Rookie Drafts: Burden profiles as an elite fantasy asset with immediate WR1/WR2 potential. His game-breaking YAC ability, versatility, and overall polish make him a high-floor, high-ceiling prospect. The RSP evaluator considers him a cornerstone talent likely being undervalued by the consensus (potentially enabling a trade-down scenario while still acquiring him). He should be considered a lock for a top-3 pick in rookie drafts, with a strong argument for being the 1.01 depending on format and team needs.</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>X – Chris Olave/Ricky Pearsall</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Travis Hunter presents perhaps the biggest risk/reward conundrum in this draft class for fantasy football managers. Evaluated here as the RSP WR2 with "Franchise" level talent, he possesses Pro-Bowl potential as a wide receiver due to his skilled route running, vertical ability, reliable hands, and good YAC skills, drawing comparisons to Chris Olave and Ricky Pearsall. HOWEVER, the massive uncertainty about his NFL position overshadows everything. The evaluator expresses skepticism about him playing both ways significantly and leans towards Hunter primarily playing Cornerback in the NFL, despite acknowledging his offensive gifts. This positional ambiguity makes drafting him for fantasy purposes before the NFL Draft clarifies his role extremely risky.
+Fantasy Strengths (as a potential WR):
+Skilled Route Running: Polished and nuanced route runner with a variety of releases (though needing more consistent pacing/artfulness vs. press), effective setups, and precise breaks. Wins vs. man coverage.
+Vertical Threat: Possesses big-play ability downfield, capable of stacking defenders and winning on intermediate-to-deep routes.
+Reliable Hands &amp; Catching: Excellent catch reliability (100% pinpoint/tight coverage catch rate in tracked games), sound technique, wins through contact, and positions himself well on contested catches.
+Good YAC Ability: Shows agility, quick deceleration, spin moves, and vision to create yards after the catch, leveraging blockers well on screens/RPOs.
+High Football IQ: Understands zone concepts, works scramble drills effectively, and shows good situational awareness as a receiver.
+Durability: No significant injuries reported despite heavy college workload (playing both ways).
+Fantasy Weaknesses/Concerns:
+Positional Uncertainty (MASSIVE RISK): The biggest factor. Will he be a WR, CB, or some limited mix? The evaluator leans CB, which would make him essentially worthless in standard fantasy formats. Drafting him pre-NFL Draft is a huge gamble on his offensive role.
+Release vs. Press: Needs refinement in pacing and technique to consistently beat physical press coverage at the NFL level. Can get pushed off his line.
+Decision-Making (YAC): Occasionally tries to do too much after the catch, leading to retreats or poor decisions instead of taking available yards (though expected to improve).
+Unnecessary Leaping: Sometimes leaves his feet unnecessarily for higher targets, potentially costing YAC opportunities.
+Player Comparisons (as a WR):
+Chris Olave / Ricky Pearsall: These comparisons highlight his potential as a smooth, skilled route runner with reliable hands and the ability to create separation.
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Drafting Travis Hunter requires extreme caution. While his talent as a receiver warrants early first-round consideration based on this profile, the significant risk that his NFL team primarily views him as a cornerback makes him a potential fantasy bust.
+If his NFL team commits to him playing WR: His fantasy value skyrockets, likely into the top half of the first round of rookie drafts.
+If his primary role is CB (or unclear): His fantasy value plummets, making him undraftable in most standard leagues. The RSP evaluator explicitly advises waiting until the 4th round of early (pre-NFL Draft) rookie drafts if you want to take a speculative gamble, highlighting the immense risk involved before his NFL role is known. His landing spot and the team's stated intentions will be paramount.</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tim Brown – X/Jayden Reed - Lee Evans – Curtis Samuel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starter: Starting immediately with a large role and learning on the go. Golden is on the 
+cusp of the Franchise Tier: Challenging for the lead role and leadership anchor. </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Matthew Golden (RSP WR3) is profiled as a dynamic, versatile wide receiver prospect poised for immediate impact, grading out on the cusp of the "Franchise" tier. Possessing elite timed speed (4.29 40-yard dash), Golden is far more than just a speedster, showcasing savvy route running that leverages his speed, reliable hands, and excellent ability after the catch. Drawing comparisons to versatile playmakers like Tim Brown and Jayden Reed, Golden can threaten defenses vertically, turn short passes into long gains, and operate effectively from multiple alignments (flanker, slot). While needing to improve consistency in contested catch situations and blocking, his overall skillset suggests high upside as potentially a primary or high-end secondary target in an NFL offense early in his career.
+Fantasy Strengths:
+Elite Speed &amp; Athleticism: Fastest timed WR in the class; possesses game-breaking speed for vertical routes and pulling away after the catch.
+Advanced Route Running: Intelligently uses his speed within routes, attacks stems effectively, shows sharp breaks with good deceleration, and understands how to set up defenders. Not just a vertical threat.
+Excellent YAC Ability: Displays quickness, vision, body control, and power after the catch to make multiple defenders miss, break tackles, and finish runs. Dangerous with the ball in his hands.
+Reliable Hands &amp; Tracking: Very dependable hands (100% catch rate on pinpoint/general targets in tracked games), tracks the ball well (including over-the-shoulder), extends effectively, and makes catches through contact.
+Versatility: Capable of playing multiple WR roles (flanker, slot) and winning in various ways (deep, intermediate, short, YAC). Viewed as a "match-up player."
+Good Ball Security: Takes care of the football with generally sound technique.
+Fantasy Weaknesses:
+Inconsistent Contested Catch Technique: While capable of making spectacular contested catches, struggles with timing, positioning, and attack technique consistently, especially when pinned near the boundary (67% tight coverage catch rate, drops vs. contact noted).
+Blocking Technique: Needs refinement; relies more on shielding/positioning ("hugger") than effective strikes, which could lead to holding penalties or ineffective blocks.
+Durability Concerns: Has a history of multiple nagging injuries (foot, groin, back) over the past couple of seasons, raising some concern about his ability to consistently stay available.
+Minor Catching Lapses: Occasional "clap-catches" on low targets need cleaning up.
+Player Comparisons:
+High end: Tim Brown (versatile HOF playmaker).
+Modern comps: Jayden Reed (versatile slot/outside threat), Lee Evans (deep threat ability), Curtis Samuel (speed/YAC/versatility). These comparisons point to a dynamic offensive weapon.
+Bottom Line for Rookie Drafts: Golden possesses an elite combination of speed, route-running savvy, reliable hands, and YAC ability, making him a high-upside fantasy prospect. He projects as an immediate contributor who can be deployed in multiple ways to exploit defenses. While he needs to improve his contested-catch consistency and blocking, his playmaking potential is significant. The RSP evaluator suggests he warrants late first-round consideration in rookie drafts (pre-NFL Draft), potentially slipping into the early second, representing strong value for a player with his dynamic profile.</t>
+  </si>
+  <si>
+    <t>Isaac Bruce – T.Y. Hilton/X – Marvin Mims</t>
+  </si>
+  <si>
+    <t>Starter: Starting immediately with a large role and learning on the go</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Isaiah Bond (RSP WR4) profiles as a high-level "Starter" tier prospect who, according to this evaluation, might be significantly undervalued relative to his teammate Matthew Golden. Bond is described as a polished route runner with legitimate deep speed, reliable hands, dangerous YAC ability, and a strong release package, drawing comparisons to T.Y. Hilton with potential to grow into an Isaac Bruce type. While needing refinement in specific catching techniques and significant development as a blocker, Bond possesses the tools to become a high-end WR2 with WR1 potential in an NFL offense, potentially exceeding public perception and offering strong value in rookie drafts.
+Fantasy Strengths:
+Advanced Route Running &amp; Separation: Polished route runner with a diverse release package, ability to stack defenders, precise breaks (with good weight drop), and understanding of leverage/setups. Wins consistently against man coverage at intermediate and deep levels.
+Deep Speed &amp; Vertical Threat: Possesses legitimate long speed to stretch the field and win vertically.
+Reliable Hands &amp; Catching: Generally dependable hands (100% pinpoint/general catch rate in tracked games), tracks the ball well, makes catches through contact, and shows ability to win contested balls, including acrobatic plays.
+Dangerous YAC Ability: Uses acceleration, vision, patience behind blocks, and curvilinear speed effectively after the catch. Decisive and athletic in space.
+Good Athleticism: Combines deep speed with effective acceleration and agility.
+Football IQ: Understands zone coverage, works scramble drills well, and demonstrates good awareness.
+Good Ball Security: Generally secure with the ball, using the proper arm and tightening carriage in traffic.
+Fantasy Weaknesses:
+Catching Technique Lapses: While mostly reliable, shows specific inconsistencies – potential "clap-attacks" with overhand position and occasional "high-low" trapping on targets at shoulder height away from his frame.
+Underdeveloped Blocking: Technique is poor; primarily shields rather than delivers effective strikes, lacks punch, and needs significant development to contribute in the run game.
+Size: Slightly undersized frame (5'11", 180 lbs) may present challenges against larger, physical corners, though he shows ability to win contested catches.
+Durability Note: Suffered a high ankle sprain late in the 2024 season, causing him to miss a playoff game.
+Player Comparisons:
+High end: Isaac Bruce (potential ceiling).
+Primary Style Comp: T.Y. Hilton (speed, deep threat, route running).
+Contextual Comp: Profiled as Marvin Mims without the route running deficiencies Mims had entering the NFL.
+Bottom Line for Rookie Drafts: Bond appears to be a potentially undervalued asset according to this profile. He possesses the route running skills, deep speed, and reliable hands to project as a highly productive NFL receiver, likely operating as a high-end WR2 with upside for more. While blocking is a weakness and minor catching technique issues need cleaning up, his overall profile is strong. The RSP evaluator suggests targeting him in the late-first or early-second round of rookie drafts (pre-NFL Draft), anticipating he might provide excellent value compared to public perception which may view him as secondary to his teammate Golden.</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>X/Nico Collins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starter: Starting immediately with a large role and learning on the go. </t>
+  </si>
+  <si>
+    <t>Tetairoa McMillan - Fantasy Football Summary
+Overall Fantasy Outlook: Tetairoa McMillan (RSP WR5) is the top prospect fitting the appealing big-bodied 'X' receiver archetype in this class, drawing a strong comparison to Nico Collins. His elite size (6'4", 219 lbs) and exceptional ability in contested catch situations ("excels at the jump up and through") provide a significant ceiling. However, the profile indicates he requires substantial technical refinement in several key areas – particularly his releases against press coverage, route running precision, and catching technique consistency – which might limit his immediate rookie production. While possessing the tools for future dominance, he's viewed as needing more development than the receivers ranked ahead of him.
+Fantasy Strengths:
+Elite Size &amp; Frame: Prototypical dimensions for an outside 'X' receiver, creating a large catch radius.
+Excellent Contested Catch Ability: Dominant in jump ball situations, using his size, body control, and positioning to win at the catch point, especially near boundaries and in the red zone.
+Good YAC Vision &amp; Creativity: Sees the field well after the catch, shows patience, creativity (including reversing field), and finds ways to work downhill.
+Physicality: Willing to use his size and strength after the catch and shows good contact balance to work through initial hits. Possesses a violent stiff arm.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Release vs. Press (Major Refinement Needed): Lacks craft, nuance, and consistent patience/suddenness in his releases. Struggles to beat press consistently and can get pinned to the boundary easily. Needs significant development here to thrive outside in the NFL.
+Route Running Polish: Doesn't always attack leverage optimally, lacks consistent explosion/snap out of breaks, and needs to be savvier navigating underneath zone coverage. Not maximizing separation potential currently.
+Catching Technique Lapses: Prone to "clap-catches" on various targets (hitches, wide extensions, sometimes high points), occasionally fails to look the ball in fully, and technique suffers when pinned to the boundary on contested catches. This inconsistency could lead to drops at the NFL level.
+Lacks Elite Suddenness (YAC): While creative, doesn't possess the high-end quickness to consistently exploit cutback lanes he sees, limiting massive YAC gains compared to more agile receivers. Can try to get "cute" instead of using his size.
+Blocking Technique: Needs refinement; prone to overextending and relies more on shielding/latching than effective strikes.
+Player Comparisons:
+Nico Collins: This comparison highlights his potential ceiling as a big-bodied 'X' receiver who can develop into a dominant player after refining his technique, similar to Collins' trajectory.
+Bottom Line for Rookie Drafts: McMillan offers the tantalizing upside associated with dominant big receivers, making him appealing for fantasy managers prioritizing that archetype. His size and contested-catch skills provide a path to red-zone relevance and big plays. However, the significant technical refinement needed, especially in releases and route running, suggests he may require patience and might not be an immediate high-volume target earner. He carries more developmental risk than the higher-ranked, more polished receivers in this RSP evaluation. The evaluator ranks him WR5 with a notable gap below the top tier, likely placing his pre-NFL Draft rookie value in the mid-to-late first round, acknowledging both the high ceiling and the required development curve.</t>
+  </si>
+  <si>
+    <t>Iowa State</t>
+  </si>
+  <si>
+    <t>X - Tee Higgins / Mike Williams</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Jayden Higgins (RSP WR6) profiles as a high-floor "Starter" tier prospect, fitting the mold of big-bodied perimeter receivers like his pro comparisons, Tee Higgins and Mike Williams. He excels at using his size (6'4", 214 lbs) to win contested catches and erase inaccuracies, making him a valuable asset near the boundaries and in the red zone. Combined with good route running and reliable hands overall, he projects as an immediate contributor with the potential to become a high-volume "possession-plus" target. His main limitations are below-average hand strength (making him vulnerable to drops when defenders contest at the catch point) and occasional lapses in zone coverage recognition.
+Fantasy Strengths:
+Excellent Size &amp; Contested Catch Ability: Uses his large frame effectively to box out defenders, high-point the football, and win in contested situations. Great body control near the boundary. Significant red zone potential.
+Good Route Running &amp; Releases: Possesses a solid release package, understands how to set up defenders, runs routes effectively, and creates separation through technique and size. Stacks defenders on vertical routes.
+Reliable Hands (Overall): Despite hand strength concerns, generally catches the ball well, makes difficult catches through contact, and adjusts to targets effectively. High catch rates in tracked games.
+Good YAC Vision &amp; Power: While not dynamically elusive, he sees the field well after the catch, uses his size and a functional stiff arm to break tackles (especially against DBs), keeps his feet moving, and finishes runs powerfully.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Below-Average Hand Strength: Vulnerable to having the ball dislodged by defenders swatting at his hands/the ball at the catch point. This is the primary limiter to him being an elite pass catcher.
+Zone Recognition Lapses: Occasionally misreads zone coverage triangles and fails to settle in the correct open space, potentially limiting effectiveness against complex NFL zone schemes initially.
+Limited YAC Elusiveness: More efficient and powerful than dynamic after the catch; not likely to make multiple defenders miss with pure agility.
+Route Break Explosiveness: Lacks elite snap/suddenness out of some breaks (hitches, short routes).
+Player Comparisons:
+Tee Higgins / Mike Williams: Excellent comparisons highlighting his potential role as a big-bodied perimeter receiver who wins downfield and in contested situations, offering significant touchdown upside.
+Bottom Line for Rookie Drafts: Higgins profiles as a relatively safe prospect with a clear path to an NFL role as a starting perimeter receiver. His size and contested-catch ability provide a valuable skillset for fantasy, especially in the red zone. While the hand strength issue caps his absolute ceiling slightly, he projects as a reliable target who should command volume. The RSP evaluator considers him a likely bet for early production and values him as a second-round rookie pick (potentially sliding to the early third) before the NFL Draft, making him a solid target for teams needing a dependable outside receiver.</t>
+  </si>
+  <si>
+    <t>TCU / LSU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael Wilson/X – Josh Palmer </t>
+  </si>
+  <si>
+    <t>Jack Bech - Fantasy Football Summary
+Overall Fantasy Outlook: Jack Bech (RSP WR7) profiles as a reliable, well-built possession receiver with a "Starter" grade, drawing comparisons to solid NFL contributors like Michael Wilson and Josh Palmer. His strengths lie in his reliable hands, ability to win through contact and in contested situations, good short-area quickness, and effective YAC ability driven by vision and power. While lacking elite long speed, his dependable nature and route-running prowess make him a high-floor prospect likely suited for a slot/flanker role. Refinement is needed in release pacing and positioning on certain types of throws, but he projects as a potential immediate contributor.
+Fantasy Strengths:
+Reliable Hands &amp; Contested Catching: Very dependable hands (100% pinpoint catch rate in tracked games), uses his body well, wins through contact, and makes catches in tight coverage. Secure target for quarterbacks.
+Good Short-Area Quickness &amp; Releases: Possesses good quickness and acceleration off the line, utilizing a variety of releases (feet-switch, stick, hesitations) to defeat press coverage potential.
+Solid Route Running: Runs sharp breaks (especially back to the QB), understands zone concepts, and uses effective setups.
+Effective YAC (Vision/Power): Shows patience, decisiveness, and good vision after the catch. Uses a functional stiff arm, keeps feet moving through contact, drags defenders, and finishes plays physically.
+Good Blocking Technique: Shows understanding and good technique as a stalk blocker (squat stance, closes gap, hand position, footwork) even if sustain needs work.
+Good Ball Security: Appears secure with the football, handling contact well.
+Fantasy Weaknesses:
+Lacks Elite Long Speed: More quick than fast; unlikely to consistently win as a vertical deep threat based purely on speed.
+Release Pacing/Refinement: While possessing various moves, needs to better incorporate pacing variations (patience/suddenness) into his releases to consistently beat NFL corners.
+Positioning on Specific Throws: Needs work adjusting and positioning his body effectively on back-shoulder throws and underthrown passes, sometimes tipping off his intention.
+Minor Catching Technique Lapses: Occasional "clap-attacks" due to wide hands, particularly on overhand catches away from his frame.
+Blocking Sustain: Needs to sustain blocks longer, especially away from the line of scrimmage.
+Durability History: Has missed time due to knee and shin injuries in the past couple of seasons, raising minor flags.
+Player Comparisons:
+Michael Wilson / Josh Palmer: These comparisons suggest a reliable WR2/WR3 type known for dependability, good hands, and effectiveness in the intermediate areas of the field.
+Bottom Line for Rookie Drafts: Bech offers a high floor as a dependable possession receiver likely to contribute early in a slot or flanker role. His strong hands, contested-catch ability, and functional YAC skills make him a safe prospect. While he lacks elite deep speed or dynamic YAC elusiveness, he profiles as a solid chain-mover and reliable target. The RSP evaluator suggests he's a good value as a third-round rookie pick before the NFL Draft, with potential to rise into the second round if he lands in a favorable situation with immediate starting potential.</t>
+  </si>
+  <si>
+    <t>Puka Nacua - X - Jermaine Kearse – Quincy Morgan</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Emeka Egbuka (RSP WR9) is evaluated as a "Starter" tier prospect with skills suited for a specific role, likely as a flanker or slot receiver operating primarily in space. His strengths lie in his ability after the catch, good deep speed, and effectiveness on linear routes across the field. However, significant concerns about inconsistent catching technique (using the wrong attack, letting the ball into his frame, drops vs. contact) and a lack of consistent sharpness in his route breaks limit his projected effectiveness against tight man coverage, on timing routes, and in contested situations. While compared situationally to Puka Nacua's role, he's explicitly noted as less skilled currently. He projects as an immediate contributor in a defined role, but may require refinement and an ideal scheme fit to reach consistent fantasy starter production.
+Fantasy Strengths:
+Strong YAC Ability: Dangerous runner after the catch, utilizing acceleration, vision, functional power (stiff arm, finishes plays), and good balance to create extra yards. Excels when catching the ball with space to operate.
+Good Speed &amp; Acceleration: Possesses the speed to win vertically, stack defenders, and pull away after the catch.
+Effective on Linear Routes/Zone: Runs routes across the field well, understands zone concepts, and has good release moves to get into his stem.
+Good Ball Security: Generally takes care of the football with sound technique.
+Willing Blocker: Shows good effort and intensity as a blocker, even if technique is inconsistent.
+Fantasy Weaknesses:
+Inconsistent Catching Technique: Significant issue. Frequently opts for the wrong hand position (e.g., underhand on chest-high targets), lets the ball into his frame unnecessarily, and seems unprepared for non-pinpoint throws, leading to drops and struggles in contested situations (low G vs. Contact % in tracked data).
+Route Break Sharpness: Often drifts or rounds off breaks, particularly on intermediate speed cuts, limiting separation against tight coverage. Needs more consistent precision and snap.
+Limited Role Projection: Seen primarily as a flanker/slot type best utilized on crossing routes or manufactured touches rather than a boundary 'X' consistently winning against press or on contested timing routes.
+Inconsistent Blocking Technique: While effortful, technique is flawed (locks arms, drops head), making him unreliable.
+Player Comparisons:
+Role/Usage Comp: Puka Nacua (but Egbuka lacks Nacua's current skill level).
+Spectrum Comps: Jermaine Kearse / Quincy Morgan (suggesting potential for productive seasons, often excelling vertically or after the catch, but perhaps lacking elite overall consistency or refinement).
+Bottom Line for Rookie Drafts: Egbuka offers appealing speed and YAC ability that could translate to fantasy points in the right system, particularly in PPR formats where volume on shorter routes can accrue value. However, the significant concerns about his catching technique and route break precision create substantial risk and may limit his ceiling, especially against better NFL defenders. He likely needs a specific scheme (like the Rams using Nacua) that maximizes his strengths in space and minimizes his weaknesses against tight coverage. The RSP evaluator suggests he's worth an early third-round rookie pick before the NFL Draft, with potential to rise slightly if he lands in an ideal offensive fit, but views him as less versatile and refined than other top WRs in the class.</t>
+  </si>
+  <si>
+    <t>Utah State</t>
+  </si>
+  <si>
+    <t>Chris Chambers - x – John Ross/Corey Coleman</t>
+  </si>
+  <si>
+    <t>Starter: Starting immediately with a large role and learning on the go. Royals is on the cusp 
+of the Rotational Starter tier: Executes at a starter level in a role playing to their strengths.</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Jalen Royals (RSP WR10) is presented as a high-risk, high-reward prospect whose evaluation is based heavily on projected development rather than current polish. The evaluator explicitly expresses concern about scoring him this high and warns against drafting him commensurate with this rank. Royals is an explosive athlete with excellent YAC ability ("Mecole Hardman with Hands") and big-play speed. However, he is currently underdeveloped as a route runner, possesses poor release technique against press coverage, shows inconsistent zone awareness, and has lapses in catching technique. A recent foot injury adds another layer of risk. His comparisons range from productive playmaker Chris Chambers to notable busts John Ross/Corey Coleman, highlighting the significant variance in his potential outcomes.
+Fantasy Strengths:
+Excellent YAC Ability: Dynamic after the catch with elite stop-start skills, efficient cuts, good vision in traffic, and creativity to make multiple defenders miss.
+Good Speed &amp; Athleticism: Possesses game-breaking speed (ran 4.42 40 post-injury, potentially faster) and quickness. Shows good acceleration and agility.
+Good Hands (Overall): Generally reliable hands capable of making plays away from his frame, high-pointing, and digging out low throws despite technical lapses.
+Potential for Development: Evaluator notes the components for route running/releases are there, just need "stitching together," suggesting improvement is projectable (though not guaranteed). Shows flashes of good setups using pace changes during stems.
+Functional Power: Runs hard, uses stiff arm, and shows ability to run through wraps and finish plays.
+Fantasy Weaknesses:
+Raw Route Running &amp; Releases: Considered "not strong by conventional standards." Release technique lacks pacing, craft, and violence, making him vulnerable to press coverage. Route breaks often lack snap and acceleration. Significant development required.
+Inconsistent Zone Awareness: Shows eyes too early, misreads zone triangles, and doesn't always know when to settle vs. keep running, leading to potential miscommunications.
+Catching Technique Lapses: Prone to "clap-attacks" on various targets (overhand, underhand, away from frame), inconsistent positioning on contested/high-point plays. Leads to drops (PP drop vs contact noted).
+Durability/Injury: Suffered a season-ending foot injury in 2024. Recovery timeline and long-term impact are concerns, despite running at the Combine.
+Ball Security Technique: While the rate isn't terrible (1 per ~106 touches), his carrying technique (loose elbow, defaults to one side) needs improvement.
+Limited College Scheme: Heavily featured on manufactured touches (screens, RPOs, crossers); needs to prove effectiveness on a full route tree.
+Player Comparisons:
+Ceiling: Chris Chambers (big-play threat).
+Floor/Bust Risk: John Ross / Corey Coleman (athletic disappointments).
+Bottom Line for Rookie Drafts: Royals is a developmental prospect with intriguing athletic upside, particularly after the catch. However, his significant technical deficiencies as a receiver (routes, releases, hands technique, zone awareness) and recent foot injury make him a very risky fantasy investment. He likely needs a specific role featuring manufactured touches early on while he develops. The RSP evaluator explicitly advises against drafting him based on his WR10 ranking/Starter score, suggesting letting him fall 1-2 rounds lower as a speculative, high-risk/high-reward gamble, acknowledging the substantial bust potential if the necessary development doesn't occur. His NFL landing spot and coaching will be crucial.</t>
+  </si>
+  <si>
+    <t>Matthew Golden – X – John Metchie – Devin Duvernay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotational Starter: Executes at a starter level in a role playing to their strengths. Noel is 
+on the cusp of the Starter tier: Starting immediately with a large role and learning on the go. </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Jaylin Noel (RSP WR12) is presented as an athletic receiver prospect with excellent quickness and acceleration, drawing comparisons to a "discount version of Matthew Golden," as well as John Metchie and Devin Duvernay. Graded as a Rotational Starter on the cusp of the Starter tier, Noel excels with the ball in his hands and shows promise as a route runner, leveraging his stop-start ability effectively. While his game needs refinement—particularly in adding nuance to his releases and improving consistency in his route breaks and catching—he possesses the tools to develop into an every-down player capable of working inside and outside. He projects as an immediate contributor, likely in a rotational role initially, with upside for more.
+Fantasy Strengths:
+Excellent Quickness &amp; Acceleration: Possesses dynamic stop-start ability and re-acceleration, which he uses effectively both as a route runner to create separation and as a ball carrier after the catch.
+Good YAC Ability: Manipulates defenders in open space, uses his blocks well, shows decisiveness, and has an effective stiff arm. Runs with adequate power through contact for his size (5'10", 194).
+Speed Potential: Evaluator notes potential for elite speed, suggesting college QB limitations may have masked his true deep threat ability. Can blow by defenders when given space.
+Route Running Potential: Shows a variety of setups, understands how to attack leverage, uses his quickness well in routes, and displays good zone awareness. Breaks are generally clean, though sometimes lack optimal snap/flatness.
+Versatility Potential: Has the tools to eventually play both inside (slot) and outside, offering scheme flexibility. Also has gadget potential (option pass noted).
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Release Refinement Needed: While possessing various moves, lacks the consistent contrast of patience and suddenness needed to reliably beat NFL press coverage without further development.
+Inconsistent Route Breaks: Execution can be sloppy at times; breaks aren't always sharp/flat, potentially limiting separation against tight coverage.
+Catching Consistency: While generally reliable and capable of making tough catches, tracked data shows several pinpoint drops (3/21) and juggles, indicating concentration can lapse.
+Stacking Ability Unproven: Potential deep speed exists, but limited evidence on tape of consistently stacking defenders vertically.
+Player Comparisons:
+Primary Comp: "Discount Matthew Golden" (similar athletic profile, slightly less refined).
+Spectrum Comps: John Metchie (quick slot type with route savvy), Devin Duvernay (speed/quickness, gadget/returner ability).
+Bottom Line for Rookie Drafts: Noel is an athletic prospect with appealing quickness, speed potential, and YAC skills, fitting the profile of a versatile playmaker. He likely needs some development, particularly refining his releases and route consistency, before commanding a full-time starting role. However, his athletic traits give him immediate contributor potential in a rotational/slot role. The RSP evaluator suggests he's a viable second-round rookie pick, potentially falling to the third, representing solid value for a player with his athletic upside and potential to grow into a significant role.</t>
+  </si>
+  <si>
+    <t>Ole Miss</t>
+  </si>
+  <si>
+    <t>Alshon Jeffery - X/Quentin Johnston – Byan Edwards</t>
+  </si>
+  <si>
+    <t>Rotational Starter: Executes at a starter level in a role playing to their strengths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall Fantasy Outlook: Tre Harris (RSP WR14) is described as a physically gifted "draftnik favorite" known for exciting contested catches and good YAC ability, drawing a ceiling comparison to Alshon Jeffery. However, this profile expresses significant caution, highlighting that Harris is currently technically raw in crucial areas and needs substantial development, similar to Terrell Owens before he became a star. His releases, route running precision, catching technique (prone to clap-attacks/wrong hand usage), and zone awareness are all inconsistent works in progress. This lack of refinement leads to bust comparisons like Quentin Johnston and Bryan Edwards. While athletic and capable of highlight plays, Harris likely begins with situational usage and needs significant coaching to potentially reach his high ceiling.
+Fantasy Strengths:
+Contested Catch Potential: Makes exciting plays on the ball in the air, adjusts reasonably well, and shows ability to win through contact when his technique holds up. Possesses good size (6'2", 205) for this role.
+Good YAC Ability: Shines after the catch with good vision to find secondary lanes, patience, and the strength/power to run through wraps and work past multiple points of contact. Uses an effective stiff arm.
+Good Athleticism: Possesses adequate speed and acceleration to create separation on vertical routes occasionally and contribute after the catch. Agile enough to make defenders miss.
+Release Variety (Raw): Has a wide range of release moves in his arsenal, indicating potential if he can add craft and pacing. Shows ability to stack defenders when he gets separation.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Raw Route Running Technique: Lacks consistent precision, snap, and acceleration into/out of breaks. Setups aren't always convincing. Struggles to consistently separate against man coverage with pure technique.
+Inconsistent Release Technique: Releases often lack craft, pacing (patience/suddenness contrast), and consistent violence/effectiveness against press coverage. Can get pinned or jammed.
+Catching Technique Lapses: Prone to "clap-attacks" (especially on high points), uses suboptimal hand positions (e.g., underhand too often), and tries to transition before securing the ball, leading to drops (multiple drops vs contact/tight coverage noted in data).
+Inconsistent Zone Awareness: Doesn't always read zone triangles correctly or know when to settle vs. continue running, leading to potential miscommunications.
+Lacks Elite Speed: Not a true burner; speed is functional but unlikely to consistently erase angles against faster NFL DBs over long distances.
+Player Comparisons:
+Ceiling: Alshon Jeffery (big-bodied, contested-catch winner).
+Floor/Bust Risk: Quentin Johnston / Bryan Edwards (physically gifted but technically unrefined disappointments).
+Bottom Line for Rookie Drafts: Harris is a high-variance prospect with undeniable physical tools and highlight-reel potential, but significant technical flaws across his game make him a risky investment requiring considerable development. He fits the profile of a player who could boom if the technique clicks, but carries substantial bust potential if it doesn't. He likely needs manufactured touches or specific vertical opportunities early on. The RSP evaluator suggests that drafting him in the early third round of rookie drafts (pre-NFL Draft) might even be reaching, indicating significant concern about his immediate readiness and overall refinement compared to his perceived hype. His value is highly dependent on coaching and development at the next level.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parker Washington/X - James Proche – Amari Rodgers – Byron Marshall</t>
+  </si>
+  <si>
+    <t>Rotational Starter</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Xavier Restrepo (RSP WR19) fits the archetype of a "classic slot receiver" whose fantasy upside appears significantly limited by athletic constraints and technical flaws. While possessing strong hands at the catch point and good YAC ability fueled by shiftiness and surprising power for his size, he lacks the necessary speed, acceleration, and route-running precision to consistently separate against NFL defenders, especially outside the slot. His catching technique also breaks down on non-pinpoint throws. Comparisons to players like Parker Washington, James Proche, and Amari Rodgers suggest a likely career path as a reserve or low-volume contributor rather than a fantasy starter. The evaluator considers him a "low-ceiling, high-floor [reserve]" option and advises against drafting him before the NFL Draft clarifies his role and potential opportunity.
+Fantasy Strengths:
+Strong Hands (at Catch Point): Reliable hands when the ball is thrown accurately, shows toughness through contact, and positions himself well. Good contested catch results when positioned properly.
+Good YAC Ability: Shifty and patient runner after the catch with good vision. Uses his stocky build (5'9", 209 lbs) effectively to break tackles and gain extra yards. More powerful than typical small slots.
+Slot Savvy: Understands how to work from the slot, find space against zone coverage, and utilize releases effective in two-way go situations.
+Good Ball Security: Appears to take care of the football; no major concerns highlighted.
+Fantasy Weaknesses:
+Lack of Speed &amp; Acceleration: Does not possess the speed to threaten vertically or consistently separate from defenders based on athleticism alone. Capped athletic ceiling.
+Imprecise Route Running: Breaks lack snap, precision, and sharp deceleration, particularly on timing routes. Drifts out of breaks and struggles to create separation against man coverage.
+Inconsistent Catching Technique (Off-Target Throws): Technique falters on throws that aren't pinpoint (high/away, low/behind), resorting to "clap-attacks" that lead to drops.
+Poor Blocking: Technique is generally poor (doesn't close gap, poor strike method, gets beaten to punch), making him ineffective as a blocker.
+Limited Role Projection: Profiles almost exclusively as a slot receiver working underneath routes.
+Durability History: Missed significant time with a foot injury in 2022.
+Player Comparisons:
+Parker Washington / James Proche / Amari Rodgers / Byron Marshall: These comparisons point towards players who primarily operate from the slot, often relying on YAC or gadget roles, and have generally had limited and inconsistent fantasy production.
+Bottom Line for Rookie Drafts: Restrepo's fantasy appeal is largely confined to deeper PPR leagues where underneath targets and some YAC can provide a baseline floor. However, his lack of athletic upside, combined with technical flaws in route running and catching (on off-target throws), severely limits his ceiling. He doesn't project as a player likely to command a high target share or produce significant fantasy numbers consistently. The RSP evaluator strongly suggests waiting until after the NFL Draft to assess his situation and considers him a poor value compared to other prospects with more upside, likely making him a late-round rookie pick at best, even in deep formats.</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Tank Dell - X - Tutu Atwell</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Tez Johnson (RSP WR22) is a highly polarizing prospect due to his extreme outlier size (5'9", 154 lbs) juxtaposed with elite short-area quickness, acceleration, and polished route-running skills for a slot receiver. While his athletic traits and YAC ability draw comparisons to players like Tank Dell and Tutu Atwell, and the evaluator argues his size might not be prohibitive citing historical examples (Gerald McNeil), it undeniably creates massive uncertainty regarding his NFL draft capital, role, and long-term durability. Compounding the size issue are significant concerns about inconsistent hands/drops and very poor blocking. Johnson possesses the skills to be a dynamic playmaker from the slot if given the chance, but the risks are substantial.
+Fantasy Strengths:
+Elite Acceleration &amp; Short-Area Quickness: Possesses top-tier burst and change-of-direction ability, crucial for separating in the short-to-intermediate areas and creating yards after the catch. Tested exceptionally well in these areas.
+Polished Route Running (Slot): Described as "sudden and artful," using a variety of releases, setups (hip shifts, pace changes, sticks), and sharp breaks (when clean) to create space underneath. Excels on scramble drills.
+Strong YAC Ability: Leverages his quickness, vision, and decisiveness effectively after the catch. Patient setting up blocks and can make multiple defenders miss. Uses stiff arm well for his size.
+Toughness: Has taken hard hits over the middle despite his frame.
+Versatile Usage: Experience playing slot, backfield, and wing suggests potential for creative deployment.
+Fantasy Weaknesses:
+Extreme Size/Weight: Historically small (154 lbs), raising major questions about durability, ability to handle NFL physicality, potential role limitations, and how NFL teams will value him (draft capital risk). This is the overriding concern.
+Inconsistent Hands/Drops: "Biggest concern... is his hands." Prone to "clap-attacks" due to wide hand positioning, leading to drops and fighting the ball. Had a multi-drop game, raising concentration/confidence questions. Tracked data shows drops and low catch rate vs contact/tight coverage.
+Very Poor Blocking: Noted as a non-blocker ("Joker... without blocking element"). Technique is poor across the board (approach, strike, sustain). Major liability.
+Limited Catch Radius/Contested Ability: Size naturally limits his catch radius. Profile notes he's strictly an "open-space player," unlikely to win contested catches consistently.
+Ball Security Technique: Elbow is loose, making ball vulnerable to being knocked out (though no rate provided).
+Durability: Shoulder injury in 2024 adds to long-term concerns given extreme weight.
+Player Comparisons:
+Tank Dell / Tutu Atwell: Undersized slot receivers known for speed/quickness, used primarily in space/gadget roles, with varying degrees of NFL success/consistency.
+Historical Comp: Gerald McNeil (used to argue against size being prohibitive, highlighting McNeil's success as a tiny returner in a tougher era).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Johnson is the ultimate boom-or-bust prospect based on whether an NFL team is willing to overlook his unprecedented size and inconsistent hands to utilize his elite quickness and route savvy from the slot. If he earns significant draft capital (inside Round 6 suggested as a benchmark by RSP) and lands with a creative play-caller, he offers intriguing upside, especially in PPR formats. However, the risks (size, drops, blocking inability) are immense. The RSP evaluator advises extreme caution, suggesting fantasy managers wait for the NFL Draft to gauge team interest before considering Johnson, likely only as a speculative pick in the second half of rookie drafts if the draft capital provides a "tacit stamp of approval."</t>
+  </si>
+  <si>
+    <t>TCU</t>
+  </si>
+  <si>
+    <t>Cordarrelle Patterson</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Savion Williams (RSP WR11) is a unique and intriguing prospect due to his potential positional ambiguity, drawing a direct comparison to Cordarrelle Patterson. Possessing an elite physical profile (6'4", 222 lbs) and exceptional ability with the ball in his hands, Williams grades out with elite power and contact balance by running back standards and has experience playing the position at TCU. While evaluated primarily as a WR here (Rotational Starter, cusp of Starter tier), his ceiling might be highest if an NFL team converts him to RB. As a receiver, he shows promising tools – good releases, attacking leverage, reliable hands – but needs refinement in pacing, route setups, and break consistency. His fantasy value is highly dependent on his declared NFL position.
+Fantasy Strengths:
+Elite Physical Tools &amp; Size: Outstanding size, power, agility, and contact balance profile.
+Exceptional Ball Carrier Ability (RB Potential): Described as one of the best YAC receivers, essentially grading as a running back with the ball. Runs through all levels of contact, shows patience/decisiveness between tackles, good footwork/hip mobility. Potential first-round rookie pick value if drafted as an RB.
+Good Release Package (Potential): Possesses a variety of moves (read step, double up, stick, counters) and attacks leverage; needs refinement in pacing/craft.
+Promising Route Running Elements: Attacks stems, shows ability to stack, executes certain breaks well (snaps turns), understands zone concepts. Good foundation but needs more polish/variety in setups.
+Reliable Hands &amp; Contested Catches: Generally dependable hands, makes difficult catches, uses size well, good focus through contact, and strong enough hands to resist defenders. Excellent tight coverage catch rate (100%).
+Physical Blocker: Willing and physical blocker who gets hands inside and keeps feet moving.
+Fantasy Weaknesses:
+Positional Uncertainty: Will he be a WR, RB, or hybrid weapon? This creates significant variance in his fantasy projection pre-NFL Draft.
+WR Technique Refinement Needed: Requires more craft/pacing on releases, needs to add route setups, inconsistent sharpness/technique on certain breaks.
+Minor Catching Lapses: Occasional focus drops, sometimes uses suboptimal hand position (underhand on number targets), rare clap-attacks over the shoulder. Drops noted in tracked data.
+Durability History: Missed significant time early in his college career due to unspecified injuries, raising minor flags despite recent health.
+Player Comparisons:
+Cordarrelle Patterson: Perfect comparison highlighting his potential as a big, athletic weapon who excels with the ball in his hands, usable as a WR, RB, or returner, but potentially needing schematic help or development to thrive purely as a traditional WR.
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Savion Williams is one of the most fascinating prospects due to his potential RB conversion upside.
+As a WR: He projects as a high-upside rotational player (WR11 rank) with good size and YAC ability, needing technical refinement but offering intriguing potential. The RSP evaluator suggests he's worth considering in the second round of rookie drafts in this role.
+As an RB: His physical tools grade out as potentially elite, offering a ceiling of 2,000 scrimmage yards and double-digit TDs according to the evaluator. If an NFL team drafts him with the intention of playing him at RB, his fantasy value would skyrocket, potentially into the first round of rookie drafts. Monitor his NFL Draft designation closely; it will dictate his fantasy value more than almost any other prospect. He's a high-upside gamble with multiple paths to fantasy relevance.</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adonai Mitchell – X – Marquez Callaway – Jaray Jenkins </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Elic Ayomanor (RSP WR24) presents a frustratingly inconsistent profile. He possesses intriguing tools, including good size (6'2", 206 lbs) and a surprisingly refined and diverse release package that often creates initial separation. However, his evaluation is marred by significant flaws after the release, particularly egregious struggles at the catch point against tight coverage due to poor technique (clap-attacks, suboptimal attack choices, poor positioning) and an inability to consistently stack defenders. This leads to a boom-bust profile with comparisons ranging from the similarly frustrating Adonai Mitchell to disappointing journeymen like Marquez Callaway and Jaray Jenkins. The evaluator expresses significant concern, suggesting Ayomanor frequently undermines his own good work and advises extreme caution in rookie drafts.
+Fantasy Strengths:
+Good Release Package: Possesses a strong array of nuanced footwork and hand counters delivered with good patience/suddenness contrast, allowing him to win early against coverage at the line.
+Good Size &amp; Frame: Has the physical dimensions desired for an outside receiver role.
+Functional YAC Ability: Uses his size and strength effectively after the catch, runs through contact, employs a decent stiff arm, and shows awareness to split defenders when needed.
+Solid Blocker: Shows good technique and willingness as a blocker in the run game.
+Good Ball Security &amp; Durability (Recently): Takes care of the ball; played full seasons recently despite past knee issues (HS PCL, 2022 camp injury).
+Fantasy Weaknesses:
+Poor Catch Point Execution vs. Tight Coverage: Major weakness. Consistently fails to secure contested catches due to poor technique ("clap-attacks"), suboptimal attack angles, poor positioning, and not attacking the ball early enough. Gets the ball ripped away frequently. Low tight coverage catch rate (50%).
+Inability to Stack/Maintain Separation: Frequently allows defenders back into the play after initially winning off the line or on the stem. Doesn't capitalize on separation created.
+Lacks Elite Speed/Acceleration: Described as having build-up speed rather than sudden burst; gets chased down by safeties and doesn't consistently pull away.
+Inconsistent Catching Technique: Prone to clap-attacking even on some easier targets, suggesting fundamental flaws in hand technique beyond just contested situations.
+Player Comparisons:
+Ceiling/Style Comp: Adonai Mitchell (physically gifted, flashes separation, frustratingly inconsistent at catch point).
+Floor/Bust Risk: Marquez Callaway / Jaray Jenkins (big-bodied receivers who didn't stick due to lack of refinement/consistency).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Ayomanor is a high-risk prospect whose promising releases are frequently negated by his failures at the catch point, especially against tight coverage. While the physical tools and initial separation ability offer a glimpse of upside, his inability to consistently finish plays makes him a significant gamble. He needs major improvement in his catching technique and consistency to become a reliable fantasy asset. The RSP evaluator expresses strong skepticism, advising fantasy managers to essentially avoid him in rookie drafts before the NFL draft unless he falls significantly (4th round or later) and higher-ranked options are gone. His landing spot and coaching environment will be critical, but the existing flaws present a major hurdle.</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chris Godwin - - Brenden Rice/X – Damon Hazelton </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Pat Bryant (RSP WR25) profiles as a technically sound, reliable possession receiver with good size (6'4", 204 lbs) whose strengths lie in setting up and executing route breaks effectively. While lacking elite top-end speed, he possesses good acceleration and stop-start quickness, which he leverages well both in routes and after the catch. His hands are generally reliable, and he navigates traffic well as a runner. However, his release package needs significant refinement (lacking nuance/pacing), and minor technical inconsistencies persist (clap-attacks, break sharpness). He projects as a high-floor WR3/WR4 type, potentially filling a flanker/big slot role, similar to a Chris Godwin mold (though perhaps less dynamic), but the evaluator advises caution pre-draft due to the capped athletic ceiling.
+Fantasy Strengths:
+Good Route Running (Setups/Breaks): Excels at setting up defenders mid-route using various techniques (head fakes, peeks, insets, stair-steps) and executing breaks effectively, particularly working back to the QB. Understands zone concepts.
+Good Acceleration &amp; Quickness: Compensates for lack of top speed with good burst and stop-start ability, aiding separation and YAC.
+Effective YAC Ability: Navigates traffic well, makes defenders miss with agility (spins, cuts), shows good vision, uses a solid stiff arm, and runs with adequate power through contact.
+Reliable Hands (Generally): Wins against tight coverage, makes catches through contact, tracks well, and extends effectively. Generally dependable despite minor technical flaws.
+Good Size &amp; Blocking: Possesses good height and frame; shows good technique and willingness as a blocker.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Lack of Top-End Speed: Unlikely to consistently win vertically or generate huge plays based on speed alone. Likely confined to underneath/intermediate work primarily.
+Release Refinement Needed: Release package lacks nuance, pacing variation (patience/suddenness), and artistry needed to consistently defeat NFL press coverage at the line.
+Inconsistent Catching Technique: Prone to minor "clap-attacks," which could be problematic despite generally good hands.
+Route Break Consistency: While generally good, breaks sometimes lack optimal sharpness/snap, especially on timing routes.
+Player Comparisons:
+High end: Chris Godwin (versatile, reliable, tough possession receiver).
+Spectrum Comps: Brenden Rice / Damon Hazelton (representing a range from solid contributor to less impactful player).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Bryant offers a safe floor as a technically sound receiver with good size and reliable hands, likely capable of carving out a role as a dependable possession target. His lack of elite speed caps his ceiling, but his quickness, YAC ability, and route savvy make him a solid prospect for a WR3/WR4 role in an NFL offense, potentially as a flanker or big slot. The RSP evaluator advises monitoring him from afar pre-draft, suggesting he's likely a late-round value pick (6th-8th round leagues) unless significant NFL draft capital indicates a clearer path to early opportunity.</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Jameson Williams – X – Quez Watkins</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Tai Felton (RSP WR26) is the definition of a boom-or-bust prospect, described as having a "high ceiling with a trap door leading to a deep drop." His allure comes from legitimate deep speed and creative, dynamic ability after the catch. However, his profile is marred by significant and critical flaws, most notably highly inconsistent hands and catching technique ("catch-point woes," frequent "clap-attacks," drops), along with raw, unrefined route running and release techniques. Comparisons to Jameson Williams and Quez Watkins aptly capture his profile: tantalizing speed offset by frustrating inconsistency. He requires significant development and carries substantial risk.
+Fantasy Strengths:
+Speed &amp; Big-Play Ability: Possesses legitimate deep speed to separate vertically and is dangerous after the catch, capable of turning short gains into long touchdowns.
+Creative YAC Ability: Agile and creative with the ball in his hands, uses stop-start quickness, spins, and vision to make defenders miss and create yardage independently.
+Route Running Potential: Shows flashes of good route running elements – sharp breaks (when clean), effective setups (using head fakes, stems), and a variety of release moves. Has the athletic tools to develop further.
+Return Specialist Potential: Implied by speed/athleticism and explicitly mentioned as a way he could earn early opportunities while developing as a receiver.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Catching Technique / Drops (Major Flaw): Hands are a significant liability. Prone to frequent "clap-attacks," uses suboptimal hand positions, lets the ball into his frame, and struggles with focus, leading to numerous drops across various target types (PP, G, vs Contact, Tight Coverage drops all noted in tracked data).
+Raw Route Running &amp; Release Technique: Lacks precision, consistency, and refinement. Releases need more pacing/craft, breaks can drift or lack optimal technique, and setups aren't always convincing. Needs significant technical development.
+Inconsistent Zone Awareness: Struggles with identifying zone triangles, knowing when to settle, and showing eyes to the QB at the right time.
+Poor Blocking: Technique needs "significant correction"; approach is flawed, prone to overextension.
+Ball Security Technique: Carries ball loose, elbow wide, prone to using wrong arm near boundary.
+Player Comparisons:
+Jameson Williams / Quez Watkins: Both comparisons highlight elite speed potential coupled with significant concerns about hands, route running consistency, and overall reliability, leading to boom/bust fantasy production.
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Felton is a high-risk developmental prospect purely for fantasy managers willing to gamble on elite speed potentially overcoming massive technical flaws. His inconsistent hands are a major red flag that could prevent him from ever earning consistent targets, regardless of his speed. He likely needs time to develop and may only contribute initially via special teams or gadget plays. The RSP evaluator strongly cautions against investing significant draft capital, suggesting he's a late-round flier only, and advises having "clear boundaries" on roster patience due to the potential for him to be a "practice hype" player who struggles in games. Wait for the NFL Draft results before considering him, and even then, temper expectations significantly.</t>
+  </si>
+  <si>
+    <t>San Jose State</t>
+  </si>
+  <si>
+    <t>Michael Wilson – X/Grant DuBose – Damon Hazelton</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Nick Nash (RSP WR28) is an intriguing developmental prospect, having converted from QB to WR full-time in 2022. He shows significant promise with nuanced release packages (effectively using patience/suddenness), good route understanding, strong hands, and excellent ability in contested catch situations due to savvy positioning. Graded as a Rotational Starter, he compares favorably to reliable possession types like Michael Wilson. However, his fantasy ceiling is likely capped by a lack of high-end long speed. He also needs refinement in consistently attacking the ball early and cleaning up minor catching technique flaws (clap-attacks). He projects as a potential WR2/3 for an NFL team down the line, offering WR2-WR4 fantasy value if he develops.
+Fantasy Strengths:
+Good Route Running &amp; Releases: Possesses a wide array of release moves and effectively uses patience/suddenness to beat coverage at the line. Understands setups, runs routes well (especially timing routes), and shows good zone awareness.
+Strong Hands &amp; Contested Catch Ability: Skilled at winning contested catches through excellent positioning ("jump up and through," pull-back). Reliable hands, extends well, catches away from frame, and shows good focus through contact. High catch rates vs contact/tight coverage.
+Good Short-Area Quickness: Displays effective acceleration and change-of-direction ability, aiding releases and separation on shorter routes.
+Effective YAC Ability: Uses vision, agility (spins, jump cuts), and functional power (stiff arm, runs through wraps) to create yards after the catch.
+Versatility &amp; Football IQ: QB background likely contributes to his understanding. Has experience playing inside (slot) and outside (X).
+Good Ball Security &amp; Durability: Takes care of the ball (technique improved after early 2024 fumble) and has no significant injury history as a WR.
+Fantasy Weaknesses:
+Lack of Long Speed: Described as having speed in the "bottom range of starter value." Unlikely to consistently win deep purely on speed or pull away for long touchdowns.
+Catching Technique Refinement: Needs to attack the ball earlier more consistently, especially on targets arriving at his numbers. Prone to occasional "clap-attacks," particularly on high points.
+Route Break Polish: Speed breaks on intermediate routes need sharper execution (drive/line steps).
+Inconsistent Blocking: Technique can be flawed (overextension, relies on shielding vs. striking consistently).
+Player Comparisons:
+High end: Michael Wilson (reliable possession receiver who earned role quickly).1   
+1.
+NFL Draft Profile: Michael Wilson, Wide Receiver, Stanford Cardinal - Sports Illustrated
+www.si.com
+Spectrum Comps: Grant DuBose / Damon Hazelton (representing lower-end outcomes for this physical archetype).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Nash is a high-floor prospect due to his advanced releases, reliable hands, and contested-catch skills. His lack of top-end speed likely relegates him to a possession role working underneath and intermediate, but he has the tools to be effective there. He projects as a dependable supporting receiver (WR2/3 on his own team) who could offer steady WR3/4 fantasy value with upside for more if he continues to develop. The RSP evaluator suggests considering him as a late-round rookie pick or waiver wire addition pre-draft, viewing him as a solid developmental prospect with a good chance to carve out a meaningful role within a couple of years.</t>
+  </si>
+  <si>
+    <t>UNLV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torry Holt – Antonio Bryant - X – Ronnie Bell- Tre Turner </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Ricky White III (RSP WR34) possesses a solid technical foundation as a route runner and generally reliable hands, but his fantasy upside appears significantly capped by a lack of NFL-caliber speed ("pedestrian") and crucial inconsistencies in his catching technique. While compared aspirationally to the technician Torry Holt, his more realistic comparisons (Ronnie Bell, Tre Turner) suggest a future as a dependable but low-ceiling contributor. His inability to consistently win with speed, combined with technique flaws leading to drops (especially "clap-attacks"), makes him a risky bet for significant fantasy production. The evaluator expresses skepticism about his upside beyond a reserve role unless significant, perhaps unlikely, improvement occurs.
+Fantasy Strengths:
+Good Route Running Fundamentals: Shows good understanding of stems, setups (using sticks, double-ups, peeks), breaks (3-step, speed breaks shallow), and working back to the ball. Strong technical foundation. Good zone awareness.
+Reliable Hands (Overall): Generally catches the ball well, tracks effectively, extends, and shows good focus through contact (100% PP Catch Rate overall, though one drop noted).
+Effective YAC Ability: Makes the first man miss with stop-start quickness and agility (stick, spin, jump cut), shows good vision, and uses functional power (stiff arm, runs through wraps) after the catch.
+Good Release Variety: Possesses a solid arsenal of release moves and counters.
+Solid Blocker: Shows good technique and effort as a blocker.
+Fantasy Weaknesses:
+Lack of Top-End Speed: Described as having speed that is "pedestrian by NFL standards," significantly limiting his ability to separate vertically or be a consistent deep threat.
+Catching Technique Flaws: "Most important thing... to address." Hands are often too wide, leading to frequent "clap-attacks" on various targets (high points, over shoulder, low/behind) and subsequent drops (drops noted in tracked data). Must be fixed to survive against NFL defenders, especially given lack of speed.
+Route Running/Release Refinement Needed: Needs better pacing and artistry in releases; breaks lack consistent snap and acceleration; needs sharper execution overall to compensate for average athleticism.
+Unnecessary Leaping: Leaves feet on catchable targets, limiting YAC.
+Ball Security Technique: Carries ball loose in open field, prone to using wrong arm.
+Player Comparisons:
+Aspirational Ceiling: Torry Holt (elite technician who overcame speed limitations - seen as unlikely for White).
+Realistic Comps: Ronnie Bell / Tre Turner (solid NFL contributors, likely WR3/4 types).
+Middle Ground/Warning: Antonio Bryant (talented but inconsistent/flawed).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): White profiles as a technically sound receiver likely limited to a possession role due to athletic constraints. The major concern is whether his inconsistent catching technique can be fixed; if not, his lack of separating speed will make it very difficult to earn targets against NFL coverage. He projects as a potential depth receiver or practice squad player initially. The RSP evaluator advises extreme caution ("Monitor from afar"), suggesting fantasy managers only consider him late in very deep rookie drafts after the NFL Draft clarifies if a team invests any meaningful capital in him. He appears to have a low fantasy ceiling.</t>
+  </si>
+  <si>
+    <t>Colorado State</t>
+  </si>
+  <si>
+    <t>Van Jefferson</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Tory Horton (RSP WR63) is evaluated as a "Reserve" tier prospect with significant flaws that likely outweigh his intriguing flashes, leading to a highly cautionary outlook. While possessing some YAC quickness and a variety of release moves, his game is plagued by sloppy route breaks, problematic catching technique (especially "clap-attacks"), and a lack of NFL-caliber speed or burst. A comparison to Van Jefferson suggests a limited ceiling as a depth receiver. Compounding these issues is a recent knee injury requiring surgery. The evaluator notes potential for improvement if major technical flaws are fixed, but expresses skepticism, advising fantasy managers to "monitor from afar" and consider him only as a deep dynasty stash contingent on glowing camp reports.
+Fantasy Strengths:
+YAC Quickness: Shows good quickness, jump cuts, and spins to make defenders miss after the catch in tight quarters. Good vision to find cutback lanes.
+Release Variety (Raw): Possesses a range of release maneuvers (stretch, two-quick, foot switch, double-up, stick, counters), suggesting a foundation for development if pacing and craft are added.
+Blocking Effort/Flashes: Shows willingness and some good technical elements (squaring up, aiming for chest, moving feet) when technique holds up.
+Fantasy Weaknesses:
+Problematic Catching Technique: Major issue. Prone to "clap-attacks" due to incorrect hand positioning (palms facing each other), allows ball into frame, struggles adjusting to non-pinpoint throws, leading to drops and unreliability. Catch rate data shows drops vs contact and tight coverage.
+Sloppy Route Running: Breaks lack consistent sharpness, snap, and proper footwork (drifting, poor line steps, balance issues). Needs significant refinement for NFL separation.
+Lack of NFL Speed/Burst: Does not possess starter-level speed or acceleration; struggles to separate vertically or pull away. Athleticism is a significant limiter.
+Raw Release Technique: Lacks consistent pacing, violence, and craft needed to make his variety of moves effective against NFL corners.
+Durability/Injury: Missed most of the 2024 season with a knee injury requiring surgery in October. Recovery and long-term impact are concerns.
+Inconsistent Blocking Execution: Prone to overextending, wide hands ("hugger"), lacks punch force.
+Player Comparisons:
+Van Jefferson: Compares to a depth receiver known more for occasional flashes than consistent production or standout traits.
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Horton is a long-shot developmental prospect with significant hurdles to overcome. His catching technique issues are particularly concerning and could prevent him from sticking in the league, regardless of other skills. Combined with athletic limitations and recovery from knee surgery, his fantasy outlook is bleak. The RSP evaluator strongly advises against using a rookie pick on him before the NFL Draft and suggests only considering him as a deep dynasty stash if unexpected positive reports about his route running and catching emerge during training camp. He carries very high bust potential.</t>
+  </si>
+  <si>
+    <t>Mike Gesicki – Ed Dickson – X - Micheal Egnew</t>
+  </si>
+  <si>
+    <t>Contributor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overall Fantasy Outlook: Terrance Ferguson (RSP TE16) profiles as a highly limited, linear athlete whose intriguing size/speed/leap potential is severely undermined by significant technical flaws and a lack of functional football fluidity. Graded as a low-end "Contributor," his comparisons range from a less reliable Mike Gesicki to outright bust Micheal Egnew. While capable on straight-line routes (seams, screens) where he can build speed, he struggles immensely with skills requiring short-area quickness or bend – releases vs. tight coverage, sharp route breaks, YAC elusiveness, and blocking adjustments. Critically, his catching technique is poor ("clap-attacks," focus drops, wrong hand usage), leading to inconsistency, especially in contested situations. The evaluator is extremely low on his NFL projection and cannot recommend drafting him for fantasy purposes.
+Fantasy Strengths:
+Linear Speed/Vertical Ability: Possesses good straight-line speed once he gets a runway and vertical leaping ability. Can generate chunk plays on schemed targets (screens, seams).
+Good Tracking (Linear Routes): Tracks the ball well over his shoulder on vertical routes when he has time/space.
+YAC Power (Linear): Uses size (6'5", 247 lbs) and momentum effectively when running downhill; has a decent stiff arm and can pull through some tackles.
+Fantasy Weaknesses:
+Lack of Fluidity/Linear Athlete: "Stiff athlete" whose lack of short-area quickness and bend limits effectiveness in releases, route breaks (especially hard breaks), creating YAC through agility, and adjusting as a blocker.
+Poor Catching Technique/Drops: Major issue. Prone to frequent "clap-attacks," uses suboptimal hand positions, lacks focus, and drops contested targets far more often than he catches them. Technique breaks down on non-pinpoint throws. Low catch rates vs contact/tight coverage.
+Limited Route Running: Struggles significantly against man coverage due to inability to create separation via releases or sharp breaks. Effectiveness largely limited to zone coverage or schemed plays.
+Poor Blocking: Consistently overextends, lacks quickness to redirect, struggles with assignments requiring agility (lead blocking, stalk blocking reactions). Significant liability.
+Limited YAC Elusiveness: Not effective with stop-start movement; relies on linear power/speed rather than agility.
+Player Comparisons:
+High end (but flawed): Mike Gesicki (less reliable hands than Gesicki).
+Low end: Ed Dickson (journeyman).
+Bust warning: Micheal Egnew (similar linear athlete who failed).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Ferguson appears to be a "highlight reel" prospect whose athletic testing might entice, but his on-field limitations, particularly his poor catching technique and lack of functional fluidity, make him a very poor bet for fantasy success. He projects as a highly specialized, likely inconsistent player at the NFL level, if he sticks at all. The RSP evaluator strongly advises against drafting him in any format, viewing him as a likely bust candidate whose linear traits won't translate effectively to the nuances of the TE position in the NFL. Avoid him in rookie drafts.
+</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George Kittle - T.J. Hockenson/Tyler Eifert/X </t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Colston Loveland ranks as the RSP TE1 and possesses the all-around skillset to become a high-end NFL starter, fitting firmly into the T.J. Hockenson tier of tight ends – a versatile weapon capable of significant receiving production while being a capable blocker. While not possessing the "chimera" level blocking/receiving combination of a Gronkowski or perhaps Kittle, Loveland excels as a route runner at all levels, is dangerous after the catch, and shows promise as a blocker (though inconsistent). He projects as a potential top-three target in his future NFL offense, offering significant fantasy value, especially in TE premium formats. His recovery from major shoulder surgery (Oct '24, expected ready late July '25) is the primary immediate concern.
+Fantasy Strengths:
+Excellent Receiving Ability: Polished route runner who can stretch the field vertically (beats safeties up seam), win intermediate routes (digs), and operate underneath. Understands zone concepts, uses effective releases/setups, and shows good nuance.
+Strong YAC Ability: Physical runner after the catch who wins collisions, gets high knees through contact, drags defenders, uses an effective stiff arm, and shows good vision/patience.
+Good Athleticism &amp; Size: Ideal TE frame (6'5", 248 lbs) combined with good speed, acceleration, and agility to win as both a receiver and ball carrier.
+Versatility: Capable of lining up inline or detached and contributing significantly as both a receiver and a blocker (when technique holds). High football IQ.
+Reliable Hands: Generally dependable hands (100% PP catch rate), tracks the ball well, high-points effectively, and makes catches through contact.
+Fantasy Weaknesses:
+Inconsistent Blocking Technique: Prone to overextending inline, inconsistent aiming points on lead blocks. Needs more consistent execution despite showing capability.
+Route Break Refinement: Needs more consistent suddenness and deeper weight drop on some breaks (drop &amp; pop, whip) to maximize separation against NFL defenders.
+Minor Catching/Ball Security Lapses: Occasional clap-attacks (underhand at back hip); habit of not securing the ball immediately after catch (led to past fumble). Needs to improve boundary footwork consistency when high-pointing. Drops noted vs contact/tight coverage.
+Shoulder Injury Recovery: Underwent significant shoulder surgery (labrum/AC joint) in October 2024; expected return by late July 2025 needs monitoring for any rookie year impact or long-term concerns.
+Player Comparisons:
+Primary Comp Tier: T.J. Hockenson (high-end receiving TE, capable blocker, top-3 offensive option).
+Stylistic Comps: George Kittle / Tyler Eifert (athletic receiving TEs with blocking ability).
+Explicit Non-Comp: Brock Bowers (evaluator notes Bowers has superior athleticism).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Loveland is a top-tier TE prospect with a well-rounded game poised for significant NFL production, likely mirroring T.J. Hockenson's fantasy impact. He offers both a high floor due to his receiving skills and blocking potential, and a considerable ceiling as a potential focal point of a passing attack. The shoulder injury recovery is the main variable for his rookie season. His fantasy draft value varies significantly by format:
+TE Premium (1.5 PPR+): Clear first-round rookie pick value.
+Standard PPR: Better value in the back half of the second round.
+Non-PPR: Value likely falls to the back half of the third round. He's a strong investment, particularly in formats that reward tight end production.</t>
+  </si>
+  <si>
+    <t>LSU</t>
+  </si>
+  <si>
+    <t>Mark Andrews / X</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Mason Taylor (RSP TE2) profiles as an elite tight end prospect with a high floor and considerable ceiling, drawing strong comparisons to Mark Andrews but possessing potentially a higher ceiling as a blocker. Evaluated as a "Starter" tier talent, Taylor is a smooth, versatile athlete who excels in all facets: refined route running, reliable hands, dynamic ability after the catch, and increasingly effective blocking. While minor technical flaws exist (ball security carriage, occasional clap-attacks), his overall skillset suggests he can be a cornerstone piece of an NFL offense, potentially outproducing more hyped TEs like Loveland depending on scheme fit and opportunity. He projects as a high-end fantasy TE1.
+Fantasy Strengths:
+Excellent Receiving Skills: Smooth route runner with a solid grasp of releases, setups, and breaks. Creates separation and makes catches at all levels. Reliable hands (92% PP catch rate), extends well, wins through contact, good focus.
+Dynamic YAC Ability: Possesses impressive curvilinear speed and vision to weave through traffic after the catch, often creating extra yards independently. Uses power and a stiff arm effectively.
+Strong Blocking Potential: Shows a high ceiling as a blocker with good technique (hand usage, counters, footwork), power (uppercut, generates force), and versatility (inline, lead, pass pro). Already effective and improving.
+Ideal Size &amp; Athleticism: Prototypical TE frame (6'5", 251 lbs) combined with smooth athleticism, good acceleration, and speed to challenge defenses vertically and after the catch.
+Scheme Versatility: Fits any offensive scheme due to his well-rounded skillset; can operate inline, detached in the slot, or even outside like Ertz/Kelce, exploiting mismatches.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Ball Security Technique: Prone to swinging the ball in the open field with a loose elbow; needs to consistently keep it tighter.
+Minor Catching Technique Lapses: Occasional "small clap-attacks" on targets high and away from his frame. Drops noted on G/G vs Contact/Tight Coverage.
+Release Pacing (Minor): Footwork on releases when detached could incorporate more patience/suddenness artistry.
+Player Comparisons:
+Primary Comp: Mark Andrews (high-end receiving TE; Taylor has better blocking potential).
+Remote Ceiling Comp: George Kittle (if speed/YAC fully translate).
+Functional Comps (Usage): Zach Ertz / Travis Kelce (ability to be used detached/exploit mismatches).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Taylor looks like a high-end, immediate impact fantasy tight end. His combination of receiving prowess, dynamic YAC ability, and strong blocking potential gives him immense upside comparable to the elite TEs in the NFL. He might be undervalued in rookie drafts compared to Loveland (or Bowers if he were in this hypothetical class) but possesses arguably similar or even greater potential depending on landing spot. He warrants consideration late in the first round or early in the second round of standard rookie drafts and likely higher in TE premium formats. He has a strong chance to become a long-term fantasy TE1.</t>
+  </si>
+  <si>
+    <t>Bowling Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brock Bowers – Sam LaPorta – X/Delanie Walker – Garrett Graham  </t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Harold Fannin Jr. (RSP TE3) presents a compelling profile strongly reminiscent of Sam LaPorta, possessing elite short-area quickness and change-of-direction ability that fuel polished route running and exceptional YAC elusiveness. Graded as a "Rotational Starter," his lack of elite long speed (4.71 40-yard dash) is considered less critical given his likely role and demonstrable on-field speed that meets NFL starter standards. While blocking needs development, Fannin excels as a receiver with reliable hands and savvy movement skills. His primary risk lies in landing with a team that doesn't utilize his 'move' TE skillset optimally. If deployed correctly, he has the potential for a LaPorta-like impact as a high-volume target.
+Fantasy Strengths:
+Elite Quickness &amp; Change of Direction: Possesses top-tier agility (Shuttle/3-Cone comparable to LaPorta), enabling sharp route breaks and elite elusiveness after the catch.
+Excellent YAC Ability: Arguably the best YAC TE in the class due to creativity, patience setting up defenders, excellent footwork, and eliminating pursuit angles. Makes defenders miss frequently.
+Polished Route Running: Understands how to manipulate coverage, uses patient/sudden releases, effective setups, precise breaks (when clean), and good zone awareness. Gets open consistently underneath and intermediate.
+Reliable Hands: Generally dependable catcher (100% PP Catch Rate), adjusts well to targets, shows good focus through contact, and attacks the ball effectively.
+Versatility: Former WR/S with experience detached; fits schemes using 'move' TEs, offering mismatch potential.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Lack of Elite Long Speed: 4.71 40-time and ~20 MPH max speed confirm he's not a true field-stretching burner, limiting deep threat ceiling compared to the most explosive TEs.
+Blocking (Needs Development): Not his calling card; needs refinement and likely added strength to be more than a situational/backside blocker. Risk of being misused if coaches prioritize this.
+Scheme Fit Risk: Potential downside if drafted by a team that doesn't utilize a 'move' TE effectively or tries to make him a primary inline blocker.
+Minor Catching Lapses: Occasional clap-attacks away from frame; tracked data shows drops versus contact and tight coverage (0% catch rate in small sample).
+Player Comparisons:
+Strong Comp/Realistic Aspiration: Sam LaPorta (skillset, athletic profile sans 40, potential usage/production).
+Spectrum Comps: Brock Bowers (aspirational top end, Fannin less explosive), Delanie Walker (productive move TE), Garrett Graham (lower-end floor).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Fannin possesses the athletic traits (quickness/agility &gt; speed) and receiving skills to potentially replicate Sam LaPorta's rookie success if—and it's a significant if—he lands in the right offensive scheme that plays to his strengths. His YAC ability and route running give him significant fantasy upside, particularly in PPR formats. While the evaluator ranks him TE3, the advice is to wait until after the NFL Draft to target him, ensuring the landing spot is conducive to his success. If the fit looks good, he could be a high-value pick likely available later than Loveland/Taylor, offering similar or potentially greater fantasy production potential. He's a prime post-draft target depending on situation.</t>
+  </si>
+  <si>
+    <t>Travis Kelce – Jared Cook – Todd Heap/X – Luke Willson – Coby Fleener</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Elijah Arroyo (RSP TE4) is described as the "eye candy" of the tight end class, possessing elite speed and athleticism for his size (6'5", 250 lbs), drawing comparisons to athletic TEs like Jared Cook or Todd Heap (with Travis Kelce being a highly aspirational, likely unreachable ceiling). However, this "Rotational Starter" graded prospect comes with significant risk due to a major injury history (ACL costing most of 2022-23, recent Senior Bowl knee injury) and considerable technical rawness. His route running lacks precision, pacing, and consistent sharpness, and his catching technique breaks down on awkward targets. While his athletic gifts offer massive upside if developed, he requires significant refinement and carries substantial bust potential.
+Fantasy Strengths:
+Elite Speed &amp; Athleticism: Considered the fastest TE in the class with speed to challenge safeties vertically and pull away in the open field. Possesses good agility and overall athleticism.
+Strong YAC Potential: Uses his speed, size, and agility effectively after the catch to run through/bounce off contact, make defenders miss, and generate chunk plays.
+Good Hands/Catching (Flashes): Shows ability to make difficult athletic catches, extend for the ball, track over the shoulder, and win through contact when technique holds up. Possesses a good catch radius.
+Blocking Potential: Shows quick hands, combativeness, understands aiming points, and flashes ability to execute specific blocks well (especially backside DEs). Potential to develop into a competent blocker.
+Ideal Size: Excellent frame for a versatile TE role.
+Fantasy Weaknesses:
+Significant Injury History: Torn ACL wiped out most of his 2022 and 2023 seasons. Suffered another knee injury at the 2024 Senior Bowl. Durability is a major concern.
+Raw Route Running: Lacks refinement. Runs routes at one speed, breaks lack consistent sharpness/precision/deceleration, setups need work. Relies on athleticism over craft currently.
+Inconsistent Catching Technique: Lacks ingrained reactions/uniform hand position on awkward targets, leading to potential drops or inefficient catches. Allows ball into frame sometimes.
+Inconsistent Blocking: Prone to overextending, misses assignments due to inefficient lateral movement, needs to improve punch/sustain ability despite flashes of good technique.
+Limited Initial Role: Likely needs specific schemed looks early on leveraging his speed; blocking role best suited for backside/stalk duties initially.
+Player Comparisons:
+Ceiling Comp: Healthier Todd Heap (Realistic). Travis Kelce (Aspirational/Unlikely).
+Stylistic/Volatility Comp: Jared Cook / Luke Willson / Coby Fleener (Athletic TEs with inconsistent production often tied to refinement/hands).
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Arroyo is a high-risk, high-reward developmental tight end. His elite athleticism offers a tantalizing ceiling, but his significant injury history and considerable technical rawness (routes, hands, blocking) make him a volatile prospect. He needs time, health, and excellent coaching to reach his potential. Fantasy managers drafting him are betting purely on athletic upside overcoming major hurdles. The RSP evaluator suggests caution, viewing him as a mid-round rookie pick after Round 2 (unless in TE premium formats where the upside is more valuable earlier) and potentially a better buy-low candidate in a year or two if development stalls initially. Given the injury history and needed refinement, drafting him early is a significant gamble.</t>
+  </si>
+  <si>
+    <t>Penn State</t>
+  </si>
+  <si>
+    <t>Dallas Clark – X/Tucker Kraft</t>
+  </si>
+  <si>
+    <t>Overall Fantasy Outlook: Tyler Warren (RSP TE5) is a physically impressive prospect whose highlight reel, featuring contested catches and powerful running (including from the backfield), has generated significant buzz. However, this profile expresses caution, ranking him below the elite tiers and highlighting substantial technical deficiencies in both blocking and route running that need significant refinement for NFL success. While possessing a potential ceiling similar to Dallas Clark if development occurs, his current game is closer to Tucker Kraft, relying more on size and aggression than nuanced technique. He projects as a rotational starter initially, likely needing time and coaching to potentially reach his ceiling as a productive fantasy TE.
+Fantasy Strengths:
+Excellent Contested Catch Ability: Wins 50/50 balls effectively using his size (6'5", 256 lbs), physicality, and good positioning/body control. A potential red zone weapon.
+Strong YAC Ability: Powerful runner after the catch ("looks like tank"), patient setting up blocks, savvy footwork, breaks tackles through strength, and finishes runs with low pad level. Effective when used on designed runs.
+Versatility (Usage): Utilized inline, detached, and uniquely in the backfield (even as a QB in short yardage) at Penn State, offering schematic flexibility.
+Adequate Athleticism: Possesses viable short-area quickness and smooth acceleration for his size, though lacks elite top-end speed.
+Durability: No significant reported injuries.
+Fantasy Weaknesses:
+Poor Blocking Technique: A major area of concern. Frequently overextends, telegraphs intentions, doesn't use hands effectively (needs to learn punch), and relies on size/aggression over technique, which is less likely to work consistently in the NFL.
+Raw Route Running: Lacks artistry and refinement. Releases lack pacing variation, setups are underdeveloped, and breaks often lack necessary sharpness, snap, or weight drop, limiting separation potential against NFL defenders.
+Catching Technique Lapses (Minor): Occasional "clap-attacks," particularly on high points or when using underhand position where overhand might be better. Needs to attack the ball earlier consistently.
+Lacks Elite Speed/Dynamism: Athleticism is good, not great ("not an elite mover"). Unlikely to generate consistent breakaway plays purely with speed.
+Player Comparisons:
+Ceiling: Dallas Clark (modern version - versatile, high-volume receiver).
+Realistic Comp/Floor: Tucker Kraft (solid contributor needing refinement).
+Production Tier: Comparable potential to David Njoku / Jonnu Smith (capable of 700-900 yards, 6-8 TDs in zone-heavy/YAC roles).
+Explicit Non-Comps: Not Kittle/Gronk or Hockenson tier.
+Bottom Line for Rookie Drafts (as of April 2, 2025 - Pre-NFL Draft): Warren offers an intriguing package of size, contested-catch ability, and YAC power, making him a high-ceiling prospect if he undergoes significant technical development. However, his current rawness in route running and blocking makes him a project. He likely needs a specific role early on (red zone specialist, H-back, schemed YAC touches) while he refines his game. The RSP evaluator warns against buying into potential pre-draft hype ("overrated in early fantasy drafts") and suggests he's a safer investment after the NFL Draft reveals his landing spot and potential role. Pre-draft, he likely falls into the mid-to-late second or early third round of rookie drafts, representing a developmental gamble on his physical tools overcoming technical deficiencies.</t>
   </si>
 </sst>
 </file>
@@ -1155,18 +1831,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G36:G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.08984375" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" customWidth="1"/>
     <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
@@ -1252,20 +1927,56 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4">
+        <v>86.4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5">
+        <v>93</v>
+      </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1294,12 +2005,30 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
+      </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7">
+        <v>85.6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1354,44 +2083,134 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10">
+        <v>89.9</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" t="s">
+        <v>214</v>
+      </c>
+      <c r="F11">
+        <v>82.7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>137</v>
+      </c>
+      <c r="E12" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12">
+        <v>91.3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>135</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>166</v>
+      </c>
+      <c r="E13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13">
+        <v>84</v>
+      </c>
+      <c r="G13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E14" t="s">
+        <v>202</v>
+      </c>
+      <c r="F14">
+        <v>88.8</v>
+      </c>
+      <c r="G14" t="s">
+        <v>203</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1420,28 +2239,82 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16">
+        <v>82.9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>140</v>
+      </c>
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17">
+        <v>87.7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F18">
+        <v>86.2</v>
+      </c>
+      <c r="G18" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1470,7 +2343,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1478,12 +2351,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" t="s">
+        <v>163</v>
+      </c>
+      <c r="F21">
+        <v>84.8</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1512,7 +2403,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1520,20 +2411,56 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F24">
+        <v>85</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>52</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>209</v>
+      </c>
+      <c r="F25">
+        <v>83.3</v>
+      </c>
+      <c r="G25" t="s">
+        <v>171</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1562,12 +2489,30 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>6</v>
       </c>
       <c r="B27" t="s">
         <v>7</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27">
+        <v>86.1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>145</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1596,20 +2541,56 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29">
+        <v>71.2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>196</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>13</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
+      </c>
+      <c r="C30">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30">
+        <v>83</v>
+      </c>
+      <c r="G30" t="s">
+        <v>171</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1638,7 +2619,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1646,12 +2627,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>20</v>
       </c>
       <c r="B33" t="s">
         <v>21</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" t="s">
+        <v>211</v>
+      </c>
+      <c r="F33">
+        <v>83.2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1732,12 +2731,30 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>29</v>
       </c>
       <c r="B37" t="s">
         <v>21</v>
+      </c>
+      <c r="C37">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E37" t="s">
+        <v>198</v>
+      </c>
+      <c r="F37">
+        <v>76.2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>199</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1766,20 +2783,56 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>34</v>
+      </c>
+      <c r="D39" t="s">
+        <v>191</v>
+      </c>
+      <c r="E39" t="s">
+        <v>192</v>
+      </c>
+      <c r="F39">
+        <v>81.2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>171</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
+      </c>
+      <c r="C40">
+        <v>11</v>
+      </c>
+      <c r="D40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E40" t="s">
+        <v>177</v>
+      </c>
+      <c r="F40">
+        <v>84.9</v>
+      </c>
+      <c r="G40" t="s">
+        <v>171</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1808,12 +2861,30 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
+      </c>
+      <c r="C42">
+        <v>22</v>
+      </c>
+      <c r="D42" t="s">
+        <v>173</v>
+      </c>
+      <c r="E42" t="s">
+        <v>174</v>
+      </c>
+      <c r="F42">
+        <v>83.1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>171</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1868,20 +2939,56 @@
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
+        <v>185</v>
+      </c>
+      <c r="E45" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45">
+        <v>82.7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>171</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46" t="s">
         <v>21</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>205</v>
+      </c>
+      <c r="E46" t="s">
+        <v>206</v>
+      </c>
+      <c r="F46">
+        <v>86.3</v>
+      </c>
+      <c r="G46" t="s">
+        <v>203</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1910,20 +3017,56 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>51</v>
       </c>
       <c r="B48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>182</v>
+      </c>
+      <c r="E48" t="s">
+        <v>183</v>
+      </c>
+      <c r="F48">
+        <v>82.8</v>
+      </c>
+      <c r="G48" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
+      </c>
+      <c r="C49">
+        <v>28</v>
+      </c>
+      <c r="D49" t="s">
+        <v>188</v>
+      </c>
+      <c r="E49" t="s">
+        <v>189</v>
+      </c>
+      <c r="F49">
+        <v>82.2</v>
+      </c>
+      <c r="G49" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
@@ -1953,13 +3096,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H49" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="RB"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H50" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adds 2023-2025 RSP Rank
</commit_message>
<xml_diff>
--- a/data/RSP_Rookies.xlsx
+++ b/data/RSP_Rookies.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28a1ee50a88aa706/python_work/Dynasty_tools/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancontino/Desktop/Dynasty_tools/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="8_{0EB90C79-FC22-4A12-A94D-9985B2A593C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2874B542-5983-48EF-95C4-A7889D38744D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A5C9F8-8259-E94B-9CBE-F7F24F9A4155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="2280" windowWidth="28800" windowHeight="15460" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14040" xr2:uid="{848F5EBF-908A-44A9-800B-7860AC94F392}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$50</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="217">
   <si>
     <t>Player</t>
   </si>
@@ -1453,6 +1453,9 @@
 Notes Brooks sees himself like Josh Jacobs (whom the evaluator links to Gore).
 Floor comparison listed is CJ Anderson (solid, productive NFL starter).
 Bottom Line for Rookie Drafts: According to this evaluation, Brooks is a potential steal. He possesses the traits of a high-volume, three-down fantasy producer available at a likely Day 3 rookie draft price (RSP suggests potentially 5th-6th round rookie pick value). His combination of vision, tackle-breaking, elite ball security, and receiving chops gives him a high floor and significant ceiling. He appears NFL-ready and could quickly outperform his draft slot. Hes presented as a prime target for value-seeking fantasy managers.</t>
+  </si>
+  <si>
+    <t>RSP 2023-2025 Rank</t>
   </si>
 </sst>
 </file>
@@ -1508,10 +1511,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1831,25 +1830,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" customWidth="1"/>
-    <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="46.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1860,22 +1860,25 @@
         <v>165</v>
       </c>
       <c r="D1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" t="s">
         <v>54</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>167</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>168</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>169</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1885,23 +1888,26 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>56</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>92.9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1911,23 +1917,26 @@
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>59</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>83.7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1937,23 +1946,26 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
         <v>118</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>119</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>86.4</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>120</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1963,23 +1975,26 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>108</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>109</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>93</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1989,23 +2004,26 @@
       <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>62</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>61</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>84.6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2015,23 +2033,26 @@
       <c r="C7">
         <v>9</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>62</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>125</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>85.6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>117</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2041,23 +2062,26 @@
       <c r="C8">
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
         <v>65</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>64</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>83.8</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2067,23 +2091,26 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>67</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>89</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2093,23 +2120,26 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>113</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>114</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>89.9</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -2119,23 +2149,26 @@
       <c r="C11">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
         <v>163</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>164</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>82.7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2145,23 +2178,26 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
         <v>111</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>112</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>91.3</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2171,23 +2207,26 @@
       <c r="C13">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
         <v>131</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>132</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>84</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -2197,23 +2236,26 @@
       <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
         <v>155</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>156</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>88.8</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>157</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -2223,23 +2265,26 @@
       <c r="C15">
         <v>8</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
         <v>68</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>69</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>84.3</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -2249,23 +2294,26 @@
       <c r="C16">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
         <v>140</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>141</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>82.9</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>133</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -2275,23 +2323,26 @@
       <c r="C17">
         <v>4</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
         <v>113</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>116</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>87.7</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2301,23 +2352,26 @@
       <c r="C18">
         <v>6</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
         <v>121</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>122</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>86.2</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -2327,23 +2381,26 @@
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
         <v>71</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>72</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>82.1</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>70</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -2351,7 +2408,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2361,23 +2418,26 @@
       <c r="C21">
         <v>12</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
         <v>121</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>129</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>84.8</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="H21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="I21" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -2387,23 +2447,26 @@
       <c r="C22">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22">
+        <v>78</v>
+      </c>
+      <c r="E22" t="s">
         <v>73</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>74</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>78</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2411,7 +2474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -2421,23 +2484,26 @@
       <c r="C24">
         <v>10</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>34</v>
+      </c>
+      <c r="E24" t="s">
         <v>126</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>127</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>85</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -2447,23 +2513,26 @@
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
         <v>160</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>161</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>83.3</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>135</v>
       </c>
-      <c r="H25" s="1" t="s">
+      <c r="I25" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -2473,23 +2542,26 @@
       <c r="C26">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s">
         <v>77</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>76</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>84.5</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="H26" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2499,23 +2571,26 @@
       <c r="C27">
         <v>7</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
         <v>123</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>124</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>86.1</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>117</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -2525,23 +2600,26 @@
       <c r="C28">
         <v>16</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <v>29</v>
+      </c>
+      <c r="E28" t="s">
         <v>79</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>80</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>82.9</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>81</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -2551,23 +2629,26 @@
       <c r="C29">
         <v>63</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>162</v>
+      </c>
+      <c r="E29" t="s">
         <v>150</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>151</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>71.2</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>152</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2577,23 +2658,26 @@
       <c r="C30">
         <v>19</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
         <v>98</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>134</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>83</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>135</v>
       </c>
-      <c r="H30" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>15</v>
       </c>
@@ -2603,23 +2687,26 @@
       <c r="C31">
         <v>28</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <v>58</v>
+      </c>
+      <c r="E31" t="s">
         <v>82</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>83</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>78.5</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>84</v>
       </c>
-      <c r="H31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2627,7 +2714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -2637,23 +2724,26 @@
       <c r="C33">
         <v>4</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
         <v>98</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>162</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>83.2</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>135</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -2663,23 +2753,26 @@
       <c r="C34">
         <v>36</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <v>80</v>
+      </c>
+      <c r="E34" t="s">
         <v>85</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>86</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>75.3</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -2689,23 +2782,26 @@
       <c r="C35">
         <v>35</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
         <v>88</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>89</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>75.400000000000006</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="I35" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>27</v>
       </c>
@@ -2715,23 +2811,26 @@
       <c r="C36">
         <v>20</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
         <v>106</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>107</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>81</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -2741,23 +2840,26 @@
       <c r="C37">
         <v>16</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <v>40</v>
+      </c>
+      <c r="E37" t="s">
         <v>136</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>153</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>76.2</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>154</v>
       </c>
-      <c r="H37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -2767,23 +2869,26 @@
       <c r="C38">
         <v>13</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
         <v>105</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>72</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>83.4</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>60</v>
       </c>
-      <c r="H38" s="1" t="s">
+      <c r="I38" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -2793,23 +2898,26 @@
       <c r="C39">
         <v>34</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s">
         <v>148</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>149</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>81.2</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>135</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>35</v>
       </c>
@@ -2819,23 +2927,26 @@
       <c r="C40">
         <v>11</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40">
+        <v>35</v>
+      </c>
+      <c r="E40" t="s">
         <v>138</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>139</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>84.9</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>135</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="I40" s="1" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -2845,23 +2956,26 @@
       <c r="C41">
         <v>23</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41">
+        <v>47</v>
+      </c>
+      <c r="E41" t="s">
         <v>102</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>103</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>80.2</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="H41" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H41" s="1" t="s">
+      <c r="I41" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2871,23 +2985,26 @@
       <c r="C42">
         <v>22</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <v>55</v>
+      </c>
+      <c r="E42" t="s">
         <v>136</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>137</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>83.1</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>135</v>
       </c>
-      <c r="H42" s="1" t="s">
+      <c r="I42" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2897,23 +3014,26 @@
       <c r="C43">
         <v>11</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43">
+        <v>18</v>
+      </c>
+      <c r="E43" t="s">
         <v>98</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>101</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>83.6</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>81</v>
       </c>
-      <c r="H43" s="1" t="s">
+      <c r="I43" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2923,23 +3043,26 @@
       <c r="C44">
         <v>4</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
         <v>98</v>
       </c>
-      <c r="E44" t="s">
+      <c r="F44" t="s">
         <v>99</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>86.4</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>100</v>
       </c>
-      <c r="H44" s="1" t="s">
+      <c r="I44" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2949,23 +3072,26 @@
       <c r="C45">
         <v>26</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45">
+        <v>61</v>
+      </c>
+      <c r="E45" t="s">
         <v>144</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>145</v>
       </c>
-      <c r="F45">
+      <c r="G45">
         <v>82.7</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>135</v>
       </c>
-      <c r="H45" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -2975,23 +3101,26 @@
       <c r="C46">
         <v>2</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
         <v>158</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>159</v>
       </c>
-      <c r="F46">
+      <c r="G46">
         <v>86.3</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>157</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -3001,23 +3130,26 @@
       <c r="C47">
         <v>24</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
         <v>91</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>93</v>
       </c>
-      <c r="F47">
+      <c r="G47">
         <v>80.099999999999994</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>51</v>
       </c>
@@ -3027,23 +3159,26 @@
       <c r="C48">
         <v>25</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48">
+        <v>59</v>
+      </c>
+      <c r="E48" t="s">
         <v>142</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>143</v>
       </c>
-      <c r="F48">
+      <c r="G48">
         <v>82.8</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>135</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -3053,23 +3188,26 @@
       <c r="C49">
         <v>28</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49">
+        <v>66</v>
+      </c>
+      <c r="E49" t="s">
         <v>146</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>147</v>
       </c>
-      <c r="F49">
+      <c r="G49">
         <v>82.2</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>135</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -3079,24 +3217,27 @@
       <c r="C50">
         <v>3</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
         <v>95</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>96</v>
       </c>
-      <c r="F50">
+      <c r="G50">
         <v>89</v>
       </c>
-      <c r="G50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>215</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H50" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
+  <autoFilter ref="A1:I50" xr:uid="{57BB6BA8-4F4C-43D2-B7ED-38D13DC00C71}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>